<commit_message>
update results, updated patty board
</commit_message>
<xml_diff>
--- a/hardware/Test result.xlsx
+++ b/hardware/Test result.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TL494 Test points" sheetId="2" r:id="rId2"/>
+    <sheet name="eletronic load reading error" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t>Initial</t>
   </si>
@@ -36,6 +38,120 @@
   </si>
   <si>
     <t>V (v)</t>
+  </si>
+  <si>
+    <t>OV test</t>
+  </si>
+  <si>
+    <t>B9</t>
+  </si>
+  <si>
+    <t>B10</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>OV test - remove 15V zener diode cathode, place potentiometer  pin 1 to gnd, pin 2 to 15V zener cathode and pin 3 to +VIN, power on and slowly turn up the potentiometer till the relay shuts down. Trip voltage should be &gt;18V</t>
+  </si>
+  <si>
+    <t>18.2V</t>
+  </si>
+  <si>
+    <t>1. Remove first the chopper mosfet</t>
+  </si>
+  <si>
+    <t>+13V rail test</t>
+  </si>
+  <si>
+    <t>+22 rail test</t>
+  </si>
+  <si>
+    <t>No mosfet</t>
+  </si>
+  <si>
+    <t>With mosfet</t>
+  </si>
+  <si>
+    <t>+5Vref test</t>
+  </si>
+  <si>
+    <t>Oscillator</t>
+  </si>
+  <si>
+    <t>6.9V</t>
+  </si>
+  <si>
+    <t>13.45V</t>
+  </si>
+  <si>
+    <t>21.8V</t>
+  </si>
+  <si>
+    <t>22.11V</t>
+  </si>
+  <si>
+    <t>5.03V</t>
+  </si>
+  <si>
+    <t>103Khz</t>
+  </si>
+  <si>
+    <t>Vout @ 150mA</t>
+  </si>
+  <si>
+    <t>Vout @ 1.5A</t>
+  </si>
+  <si>
+    <t>14.02V</t>
+  </si>
+  <si>
+    <t>14.06V</t>
+  </si>
+  <si>
+    <t>V-Batt</t>
+  </si>
+  <si>
+    <t>49.33V</t>
+  </si>
+  <si>
+    <t>49.66V</t>
+  </si>
+  <si>
+    <t>18.65V</t>
+  </si>
+  <si>
+    <t>21.62V</t>
+  </si>
+  <si>
+    <t>5.036V</t>
+  </si>
+  <si>
+    <t>105.8Khz</t>
+  </si>
+  <si>
+    <t>13.43V</t>
+  </si>
+  <si>
+    <t>21.72V</t>
+  </si>
+  <si>
+    <t>14.01V</t>
+  </si>
+  <si>
+    <t>150mA</t>
+  </si>
+  <si>
+    <t>300mA+</t>
+  </si>
+  <si>
+    <t>Pulsing/Unregulated below</t>
+  </si>
+  <si>
+    <t>Fluke</t>
+  </si>
+  <si>
+    <t>Electronic Load (mA)</t>
   </si>
 </sst>
 </file>
@@ -82,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -97,6 +213,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -114,6 +236,1022 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'eletronic load reading error'!$A$3:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'eletronic load reading error'!$B$3:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'eletronic load reading error'!$A$3:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'eletronic load reading error'!$C$3:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>485</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>727</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>968</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1213</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1455</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="652578272"/>
+        <c:axId val="652586976"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="652578272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="652586976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="652586976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="652578272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -381,7 +1519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -617,4 +1755,274 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="H5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="H5:I5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W22" sqref="W22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>150</v>
+      </c>
+      <c r="B3" s="1">
+        <v>150</v>
+      </c>
+      <c r="C3" s="1">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>200</v>
+      </c>
+      <c r="B4" s="1">
+        <v>200</v>
+      </c>
+      <c r="C4" s="1">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>500</v>
+      </c>
+      <c r="B5" s="1">
+        <v>500</v>
+      </c>
+      <c r="C5" s="1">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>750</v>
+      </c>
+      <c r="B6" s="1">
+        <v>750</v>
+      </c>
+      <c r="C6" s="1">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1000</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C7" s="1">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1250</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1250</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1500</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1500</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1455</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test result updated for electronic load reading, changed meter user to master user for testing only
</commit_message>
<xml_diff>
--- a/hardware/Test result.xlsx
+++ b/hardware/Test result.xlsx
@@ -198,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -219,6 +219,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -293,7 +296,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -314,33 +317,141 @@
             </a:effectLst>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'eletronic load reading error'!$A$3:$A$9</c:f>
+              <c:f>'eletronic load reading error'!$A$3:$A$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="9">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="14">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="19">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>1250</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="24">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1450</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>1500</c:v>
                 </c:pt>
               </c:numCache>
@@ -348,35 +459,77 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'eletronic load reading error'!$B$3:$B$9</c:f>
+              <c:f>'eletronic load reading error'!$B$3:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="9">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="14">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="23">
                   <c:v>1250</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="28">
                   <c:v>1500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -397,33 +550,141 @@
             </a:effectLst>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'eletronic load reading error'!$A$3:$A$9</c:f>
+              <c:f>'eletronic load reading error'!$A$3:$A$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="9">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>750</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="14">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="19">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>1250</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="24">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1450</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>1500</c:v>
                 </c:pt>
               </c:numCache>
@@ -431,35 +692,77 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'eletronic load reading error'!$C$3:$C$9</c:f>
+              <c:f>'eletronic load reading error'!$C$3:$C$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>143</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>192</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>485</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>727</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>968</c:v>
+                  <c:v>289</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>337</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>386</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>433</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>482</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>531</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>579</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>627</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>676</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>724</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>772</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>820</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>869</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>918</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>966</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>1213</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="28">
                   <c:v>1455</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -469,11 +772,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="652578272"/>
-        <c:axId val="652586976"/>
+        <c:axId val="351973472"/>
+        <c:axId val="351975648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="652578272"/>
+        <c:axId val="351973472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -527,12 +830,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="652586976"/>
+        <c:crossAx val="351975648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="652586976"/>
+        <c:axId val="351975648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -586,7 +889,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="652578272"/>
+        <c:crossAx val="351973472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -615,6 +918,9 @@
         <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
               <a:solidFill>
                 <a:schemeClr val="lt1">
                   <a:lumMod val="75000"/>
@@ -1231,8 +1537,8 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1793,14 +2099,14 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="H5" s="6" t="s">
+      <c r="E5" s="8"/>
+      <c r="H5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="6"/>
+      <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
@@ -1925,10 +2231,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C9"/>
+  <dimension ref="A2:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W22" sqref="W22"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1946,78 +2252,276 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>150</v>
-      </c>
-      <c r="B3" s="1">
-        <v>150</v>
-      </c>
-      <c r="C3" s="1">
-        <v>143</v>
+        <v>100</v>
+      </c>
+      <c r="B3" s="6">
+        <v>100</v>
+      </c>
+      <c r="C3" s="6">
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="B4" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="C4" s="1">
-        <v>192</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="B5" s="1">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="C5" s="1">
-        <v>485</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>750</v>
-      </c>
-      <c r="B6" s="1">
-        <v>750</v>
-      </c>
-      <c r="C6" s="1">
-        <v>727</v>
+        <v>250</v>
+      </c>
+      <c r="B6" s="6">
+        <v>250</v>
+      </c>
+      <c r="C6" s="6">
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1000</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1000</v>
-      </c>
-      <c r="C7" s="1">
-        <v>968</v>
+        <v>300</v>
+      </c>
+      <c r="B7" s="6">
+        <v>300</v>
+      </c>
+      <c r="C7" s="6">
+        <v>289</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1250</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1250</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1213</v>
+        <v>350</v>
+      </c>
+      <c r="B8" s="6">
+        <v>350</v>
+      </c>
+      <c r="C8" s="6">
+        <v>337</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>400</v>
+      </c>
+      <c r="B9" s="6">
+        <v>400</v>
+      </c>
+      <c r="C9" s="6">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>450</v>
+      </c>
+      <c r="B10" s="6">
+        <v>450</v>
+      </c>
+      <c r="C10" s="6">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>500</v>
+      </c>
+      <c r="B11" s="1">
+        <v>500</v>
+      </c>
+      <c r="C11" s="1">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>550</v>
+      </c>
+      <c r="B12" s="6">
+        <v>550</v>
+      </c>
+      <c r="C12" s="6">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>600</v>
+      </c>
+      <c r="B13" s="6">
+        <v>600</v>
+      </c>
+      <c r="C13" s="6">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>650</v>
+      </c>
+      <c r="B14" s="6">
+        <v>650</v>
+      </c>
+      <c r="C14" s="6">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>700</v>
+      </c>
+      <c r="B15" s="6">
+        <v>700</v>
+      </c>
+      <c r="C15" s="6">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>750</v>
+      </c>
+      <c r="B16" s="1">
+        <v>750</v>
+      </c>
+      <c r="C16" s="1">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>800</v>
+      </c>
+      <c r="B17" s="6">
+        <v>800</v>
+      </c>
+      <c r="C17" s="6">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>850</v>
+      </c>
+      <c r="B18" s="6">
+        <v>850</v>
+      </c>
+      <c r="C18" s="6">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>900</v>
+      </c>
+      <c r="B19" s="6">
+        <v>900</v>
+      </c>
+      <c r="C19" s="6">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>950</v>
+      </c>
+      <c r="B20" s="6">
+        <v>950</v>
+      </c>
+      <c r="C20" s="6">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1000</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C21" s="1">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1050</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1100</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1250</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1250</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>1500</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B31" s="1">
         <v>1500</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C31" s="1">
         <v>1455</v>
       </c>
     </row>

</xml_diff>

<commit_message>
separated released firmware folder
</commit_message>
<xml_diff>
--- a/hardware/Test result.xlsx
+++ b/hardware/Test result.xlsx
@@ -198,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -219,6 +219,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -520,8 +523,32 @@
                 <c:pt idx="18">
                   <c:v>1000</c:v>
                 </c:pt>
+                <c:pt idx="19">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1200</c:v>
+                </c:pt>
                 <c:pt idx="23">
                   <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1450</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>1500</c:v>
@@ -697,67 +724,91 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>96</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>143</c:v>
+                  <c:v>151</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>192</c:v>
+                  <c:v>201</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>240</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>289</c:v>
+                  <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>337</c:v>
+                  <c:v>347</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>386</c:v>
+                  <c:v>401</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>433</c:v>
+                  <c:v>453</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>482</c:v>
+                  <c:v>505</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>531</c:v>
+                  <c:v>557</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>579</c:v>
+                  <c:v>609</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>627</c:v>
+                  <c:v>660</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>676</c:v>
+                  <c:v>711</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>724</c:v>
+                  <c:v>762</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>772</c:v>
+                  <c:v>813</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>820</c:v>
+                  <c:v>865</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>869</c:v>
+                  <c:v>916</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>918</c:v>
+                  <c:v>966</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>966</c:v>
+                  <c:v>1016</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1067</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1119</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1170</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1221</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1213</c:v>
+                  <c:v>1272</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1323</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1374</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1425</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1475</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1455</c:v>
+                  <c:v>1527</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -772,11 +823,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="351973472"/>
-        <c:axId val="351975648"/>
+        <c:axId val="-592101328"/>
+        <c:axId val="-592097520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="351973472"/>
+        <c:axId val="-592101328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -830,12 +881,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="351975648"/>
+        <c:crossAx val="-592097520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="351975648"/>
+        <c:axId val="-592097520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -889,7 +940,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="351973472"/>
+        <c:crossAx val="-592101328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2099,14 +2150,14 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="H5" s="8" t="s">
+      <c r="E5" s="9"/>
+      <c r="H5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="8"/>
+      <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
@@ -2234,7 +2285,7 @@
   <dimension ref="A2:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2258,7 +2309,7 @@
         <v>100</v>
       </c>
       <c r="C3" s="6">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2269,7 +2320,7 @@
         <v>150</v>
       </c>
       <c r="C4" s="1">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2280,7 +2331,7 @@
         <v>200</v>
       </c>
       <c r="C5" s="1">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2291,7 +2342,7 @@
         <v>250</v>
       </c>
       <c r="C6" s="6">
-        <v>240</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2302,7 +2353,7 @@
         <v>300</v>
       </c>
       <c r="C7" s="6">
-        <v>289</v>
+        <v>302</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2313,7 +2364,7 @@
         <v>350</v>
       </c>
       <c r="C8" s="6">
-        <v>337</v>
+        <v>347</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2324,7 +2375,7 @@
         <v>400</v>
       </c>
       <c r="C9" s="6">
-        <v>386</v>
+        <v>401</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2335,7 +2386,7 @@
         <v>450</v>
       </c>
       <c r="C10" s="6">
-        <v>433</v>
+        <v>453</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2346,7 +2397,7 @@
         <v>500</v>
       </c>
       <c r="C11" s="1">
-        <v>482</v>
+        <v>505</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2357,7 +2408,7 @@
         <v>550</v>
       </c>
       <c r="C12" s="6">
-        <v>531</v>
+        <v>557</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2368,7 +2419,7 @@
         <v>600</v>
       </c>
       <c r="C13" s="6">
-        <v>579</v>
+        <v>609</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2379,7 +2430,7 @@
         <v>650</v>
       </c>
       <c r="C14" s="6">
-        <v>627</v>
+        <v>660</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2390,7 +2441,7 @@
         <v>700</v>
       </c>
       <c r="C15" s="6">
-        <v>676</v>
+        <v>711</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2401,7 +2452,7 @@
         <v>750</v>
       </c>
       <c r="C16" s="1">
-        <v>724</v>
+        <v>762</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2412,7 +2463,7 @@
         <v>800</v>
       </c>
       <c r="C17" s="6">
-        <v>772</v>
+        <v>813</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2423,7 +2474,7 @@
         <v>850</v>
       </c>
       <c r="C18" s="6">
-        <v>820</v>
+        <v>865</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2434,7 +2485,7 @@
         <v>900</v>
       </c>
       <c r="C19" s="6">
-        <v>869</v>
+        <v>916</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2445,7 +2496,7 @@
         <v>950</v>
       </c>
       <c r="C20" s="6">
-        <v>918</v>
+        <v>966</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2456,32 +2507,52 @@
         <v>1000</v>
       </c>
       <c r="C21" s="1">
-        <v>966</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1050</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
+      <c r="B22" s="6">
+        <v>1050</v>
+      </c>
+      <c r="C22" s="6">
+        <v>1067</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1100</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
+      <c r="B23" s="6">
+        <v>1100</v>
+      </c>
+      <c r="C23" s="6">
+        <v>1119</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1150</v>
       </c>
+      <c r="B24" s="8">
+        <v>1150</v>
+      </c>
+      <c r="C24" s="8">
+        <v>1170</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1200</v>
       </c>
+      <c r="B25" s="8">
+        <v>1200</v>
+      </c>
+      <c r="C25" s="8">
+        <v>1221</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -2491,28 +2562,52 @@
         <v>1250</v>
       </c>
       <c r="C26" s="1">
-        <v>1213</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1300</v>
       </c>
+      <c r="B27" s="8">
+        <v>1300</v>
+      </c>
+      <c r="C27" s="8">
+        <v>1323</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1350</v>
       </c>
+      <c r="B28" s="8">
+        <v>1350</v>
+      </c>
+      <c r="C28" s="8">
+        <v>1374</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1400</v>
       </c>
+      <c r="B29" s="8">
+        <v>1400</v>
+      </c>
+      <c r="C29" s="8">
+        <v>1425</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1450</v>
       </c>
+      <c r="B30" s="8">
+        <v>1450</v>
+      </c>
+      <c r="C30" s="8">
+        <v>1475</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -2522,7 +2617,7 @@
         <v>1500</v>
       </c>
       <c r="C31" s="1">
-        <v>1455</v>
+        <v>1527</v>
       </c>
     </row>
   </sheetData>

</xml_diff>